<commit_message>
Añadir Paginacion a la Grid de excel Inventor
</commit_message>
<xml_diff>
--- a/App.LM.Presentacion.Wpf/Resources/Setting/SettingApp.xlsx
+++ b/App.LM.Presentacion.Wpf/Resources/Setting/SettingApp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\WPF\AppListaMateriales\App.LM\App.LM.Presentacion.Wpf\Resources\Setting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A1FDC4-6F38-444B-8FE8-A0A0F6E7BE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820AD942-CE53-4190-8FC1-5065DAB22774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
   <si>
     <t>ColumnasExcelInventor</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Tipo de componente</t>
   </si>
   <si>
-    <t>Asociacion</t>
-  </si>
-  <si>
     <t>DIN-1 Pasadores cónicos</t>
   </si>
   <si>
@@ -571,6 +568,30 @@
   </si>
   <si>
     <t>Longitud</t>
+  </si>
+  <si>
+    <t>RutasArchivo</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>Inventor</t>
+  </si>
+  <si>
+    <t>C:\\Users\\myb19\\Desktop\\ID011 LM Horno Estructurado.xlsx</t>
+  </si>
+  <si>
+    <t>Maestro</t>
+  </si>
+  <si>
+    <t>C:\\Users\\myb19\\Desktop\\Maestro Productos Molecor TECH.xlsx</t>
+  </si>
+  <si>
+    <t>Navision</t>
+  </si>
+  <si>
+    <t>Sap</t>
   </si>
 </sst>
 </file>
@@ -784,17 +805,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{925C9BE9-A9EB-4A1C-9A13-A95B7A1791DD}" name="Inventor" displayName="Inventor" ref="A1:B9" totalsRowShown="0">
-  <autoFilter ref="A1:B9" xr:uid="{925C9BE9-A9EB-4A1C-9A13-A95B7A1791DD}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{925C9BE9-A9EB-4A1C-9A13-A95B7A1791DD}" name="Inventor" displayName="Inventor" ref="A1:A9" totalsRowShown="0">
+  <autoFilter ref="A1:A9" xr:uid="{925C9BE9-A9EB-4A1C-9A13-A95B7A1791DD}"/>
+  <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{47EC8DEA-A4E6-42D8-973F-ECB79AE8EDDD}" name="ColumnasExcelInventor"/>
-    <tableColumn id="2" xr3:uid="{C33227E9-BC5B-4007-9576-9854254FE0E5}" name="Asociacion"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC948D35-CEB9-493D-8C0F-D0589F47B893}" name="RutasArcchivos" displayName="RutasArcchivos" ref="C1:D5" totalsRowShown="0">
+  <autoFilter ref="C1:D5" xr:uid="{AC948D35-CEB9-493D-8C0F-D0589F47B893}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{F7664168-030D-4243-8197-46C70C8C3778}" name="RutasArchivo"/>
+    <tableColumn id="2" xr3:uid="{643F1E84-BA01-472F-AD72-474A7C838473}" name="Direccion"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDEF7D1F-9817-4576-AE03-BC1D068F8FE2}" name="DIN_TORNILLERIA" displayName="DIN_TORNILLERIA" ref="A1:E164" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E164" xr:uid="{DDEF7D1F-9817-4576-AE03-BC1D068F8FE2}"/>
   <tableColumns count="5">
@@ -1079,94 +1110,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1188,24 +1218,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" t="s">
         <v>173</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>174</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" t="s">
         <v>175</v>
-      </c>
-      <c r="D1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1226,7 +1256,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1247,7 +1277,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1268,7 +1298,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1289,7 +1319,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1310,7 +1340,7 @@
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1331,7 +1361,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1352,7 +1382,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1373,7 +1403,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1394,7 +1424,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1415,7 +1445,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1436,7 +1466,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1457,7 +1487,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1478,7 +1508,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1499,7 +1529,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1520,7 +1550,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1541,7 +1571,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1562,7 +1592,7 @@
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1583,7 +1613,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1604,7 +1634,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1625,7 +1655,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1646,7 +1676,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1667,7 +1697,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1688,7 +1718,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1709,28 +1739,28 @@
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="2">
+        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>8</v>
+      </c>
+      <c r="C26" s="2" t="str">
+        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
+        <v xml:space="preserve">DIN-259 </v>
+      </c>
+      <c r="D26" s="2">
+        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>87</v>
+      </c>
+      <c r="E26" s="2" t="str">
+        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
+        <v>Rosca de tubo Withworth; rosca interior y exterior cilíndrica medidas nominales</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B26" s="2">
-        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>8</v>
-      </c>
-      <c r="C26" s="2" t="str">
-        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
-        <v xml:space="preserve">DIN-259 </v>
-      </c>
-      <c r="D26" s="2">
-        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>87</v>
-      </c>
-      <c r="E26" s="2" t="str">
-        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
-        <v>Rosca de tubo Withworth; rosca interior y exterior cilíndrica medidas nominales</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="B27" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1751,7 +1781,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1772,7 +1802,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1793,7 +1823,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1814,7 +1844,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1835,7 +1865,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1856,7 +1886,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1877,28 +1907,28 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="2">
+        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>8</v>
+      </c>
+      <c r="C34" s="2" t="str">
+        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
+        <v xml:space="preserve">DIN-405 </v>
+      </c>
+      <c r="D34" s="2">
+        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>43</v>
+      </c>
+      <c r="E34" s="2" t="str">
+        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
+        <v>Rosca redonda. Forma y dimensiones.</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B34" s="2">
-        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>8</v>
-      </c>
-      <c r="C34" s="2" t="str">
-        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
-        <v xml:space="preserve">DIN-405 </v>
-      </c>
-      <c r="D34" s="2">
-        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>43</v>
-      </c>
-      <c r="E34" s="2" t="str">
-        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
-        <v>Rosca redonda. Forma y dimensiones.</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="B35" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1919,7 +1949,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1940,7 +1970,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1961,7 +1991,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1982,7 +2012,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2003,7 +2033,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2024,7 +2054,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2045,7 +2075,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B42" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2066,7 +2096,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2087,7 +2117,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B44" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2108,7 +2138,7 @@
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2129,7 +2159,7 @@
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2150,7 +2180,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B47" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2169,51 +2199,51 @@
         <v>Tornillo de cuello cilíndrico</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B48" s="2">
+        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>8</v>
+      </c>
+      <c r="C48" s="2" t="str">
+        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
+        <v xml:space="preserve">DIN-513 </v>
+      </c>
+      <c r="D48" s="2">
+        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>53</v>
+      </c>
+      <c r="E48" s="2" t="str">
+        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
+        <v>Rosca dientes de sierra. Forma y dimensiones.</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B48" s="2">
-        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>8</v>
-      </c>
-      <c r="C48" s="2" t="str">
-        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
-        <v xml:space="preserve">DIN-513 </v>
-      </c>
-      <c r="D48" s="2">
+      <c r="B49" s="2">
+        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>8</v>
+      </c>
+      <c r="C49" s="2" t="str">
+        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
+        <v xml:space="preserve">DIN-514 </v>
+      </c>
+      <c r="D49" s="2">
         <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
         <v>53</v>
       </c>
-      <c r="E48" s="2" t="str">
+      <c r="E49" s="2" t="str">
         <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
         <v>Rosca dientes de sierra. Forma y dimensiones.</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B49" s="2">
-        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>8</v>
-      </c>
-      <c r="C49" s="2" t="str">
-        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
-        <v xml:space="preserve">DIN-514 </v>
-      </c>
-      <c r="D49" s="2">
-        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>53</v>
-      </c>
-      <c r="E49" s="2" t="str">
-        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
-        <v>Rosca dientes de sierra. Forma y dimensiones.</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="B50" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2234,7 +2264,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B51" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2255,7 +2285,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B52" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2276,7 +2306,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B53" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2297,7 +2327,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B54" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2318,7 +2348,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B55" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2339,7 +2369,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B56" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2360,7 +2390,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2381,7 +2411,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B58" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2402,7 +2432,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B59" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2423,7 +2453,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2444,7 +2474,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2465,7 +2495,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2486,7 +2516,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2507,7 +2537,7 @@
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2528,7 +2558,7 @@
     </row>
     <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2549,7 +2579,7 @@
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2570,28 +2600,28 @@
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" s="2">
+        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>8</v>
+      </c>
+      <c r="C67" s="2" t="str">
+        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
+        <v xml:space="preserve">DIN-912 </v>
+      </c>
+      <c r="D67" s="2">
+        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>71</v>
+      </c>
+      <c r="E67" s="2" t="str">
+        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
+        <v>Tornillos de cabeza cilíndrica con hexágono interior tipo Allen</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B67" s="2">
-        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>8</v>
-      </c>
-      <c r="C67" s="2" t="str">
-        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
-        <v xml:space="preserve">DIN-912 </v>
-      </c>
-      <c r="D67" s="2">
-        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>71</v>
-      </c>
-      <c r="E67" s="2" t="str">
-        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
-        <v>Tornillos de cabeza cilíndrica con hexágono interior tipo Allen</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="B68" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2612,7 +2642,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2633,7 +2663,7 @@
     </row>
     <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2654,7 +2684,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2675,7 +2705,7 @@
     </row>
     <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2696,7 +2726,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2717,7 +2747,7 @@
     </row>
     <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2738,7 +2768,7 @@
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2759,7 +2789,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2780,7 +2810,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B77" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2801,7 +2831,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B78" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2822,7 +2852,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B79" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2843,7 +2873,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B80" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2864,7 +2894,7 @@
     </row>
     <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B81" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2885,7 +2915,7 @@
     </row>
     <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B82" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2906,7 +2936,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B83" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2927,7 +2957,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B84" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2948,7 +2978,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B85" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2969,7 +2999,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B86" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2990,7 +3020,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B87" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3011,7 +3041,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B88" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3032,7 +3062,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B89" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3053,7 +3083,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B90" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3074,7 +3104,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B91" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3095,7 +3125,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B92" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3116,7 +3146,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B93" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3137,7 +3167,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B94" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3158,7 +3188,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B95" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3179,7 +3209,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B96" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3200,7 +3230,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B97" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3221,7 +3251,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B98" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3242,7 +3272,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B99" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3263,7 +3293,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B100" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3284,7 +3314,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B101" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3305,7 +3335,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B102" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3326,7 +3356,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B103" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3347,7 +3377,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B104" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3368,7 +3398,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B105" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3389,7 +3419,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B106" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3410,7 +3440,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B107" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3431,7 +3461,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B108" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3452,7 +3482,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B109" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3473,7 +3503,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B110" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3494,7 +3524,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B111" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3515,7 +3545,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B112" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3536,7 +3566,7 @@
     </row>
     <row r="113" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B113" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3557,7 +3587,7 @@
     </row>
     <row r="114" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B114" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3578,7 +3608,7 @@
     </row>
     <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B115" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3599,7 +3629,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B116" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3620,28 +3650,28 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B117" s="2">
+        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>9</v>
+      </c>
+      <c r="C117" s="2" t="str">
+        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
+        <v xml:space="preserve">DIN-5463 </v>
+      </c>
+      <c r="D117" s="2">
+        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>52</v>
+      </c>
+      <c r="E117" s="2" t="str">
+        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
+        <v>Acoplamiento de ejes nervados. Serie media.</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B117" s="2">
-        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>9</v>
-      </c>
-      <c r="C117" s="2" t="str">
-        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
-        <v xml:space="preserve">DIN-5463 </v>
-      </c>
-      <c r="D117" s="2">
-        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>52</v>
-      </c>
-      <c r="E117" s="2" t="str">
-        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
-        <v>Acoplamiento de ejes nervados. Serie media.</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="B118" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3662,7 +3692,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B119" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3683,7 +3713,7 @@
     </row>
     <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B120" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3704,7 +3734,7 @@
     </row>
     <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B121" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3725,7 +3755,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B122" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3746,7 +3776,7 @@
     </row>
     <row r="123" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B123" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3767,7 +3797,7 @@
     </row>
     <row r="124" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B124" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3788,7 +3818,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B125" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3809,7 +3839,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B126" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3830,7 +3860,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B127" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3851,7 +3881,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B128" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3872,7 +3902,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B129" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3893,7 +3923,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B130" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3914,7 +3944,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B131" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3935,7 +3965,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B132" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3956,7 +3986,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B133" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3977,7 +4007,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B134" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3998,7 +4028,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B135" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4019,7 +4049,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B136" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4040,7 +4070,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B137" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4061,7 +4091,7 @@
     </row>
     <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B138" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4082,7 +4112,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B139" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4103,7 +4133,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B140" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4124,7 +4154,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B141" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4145,7 +4175,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B142" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4166,7 +4196,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B143" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4187,7 +4217,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B144" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4208,7 +4238,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B145" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4229,7 +4259,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B146" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4250,7 +4280,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B147" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4271,7 +4301,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B148" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4292,7 +4322,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B149" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4313,7 +4343,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B150" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4334,7 +4364,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B151" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4355,7 +4385,7 @@
     </row>
     <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B152" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4376,7 +4406,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B153" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4397,7 +4427,7 @@
     </row>
     <row r="154" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B154" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4418,7 +4448,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B155" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4439,7 +4469,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B156" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4460,7 +4490,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B157" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4481,7 +4511,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B158" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4502,7 +4532,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B159" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4523,7 +4553,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B160" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4544,7 +4574,7 @@
     </row>
     <row r="161" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B161" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4565,7 +4595,7 @@
     </row>
     <row r="162" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B162" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4586,7 +4616,7 @@
     </row>
     <row r="163" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B163" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4607,7 +4637,7 @@
     </row>
     <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B164" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>

</xml_diff>

<commit_message>
Actualizacion repositorySetting de excel
</commit_message>
<xml_diff>
--- a/App.LM.Presentacion.Wpf/Resources/Setting/SettingApp.xlsx
+++ b/App.LM.Presentacion.Wpf/Resources/Setting/SettingApp.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\WPF\AppListaMateriales\App.LM\App.LM.Presentacion.Wpf\Resources\Setting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820AD942-CE53-4190-8FC1-5065DAB22774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901BB6F5-CBD5-4890-81FE-F1F7D83A7AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17505" yWindow="2505" windowWidth="11265" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setting" sheetId="1" r:id="rId1"/>
-    <sheet name="Tornilleria" sheetId="2" r:id="rId2"/>
+    <sheet name="Rutas" sheetId="3" r:id="rId2"/>
+    <sheet name="Tornilleria" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
   <si>
     <t>ColumnasExcelInventor</t>
   </si>
@@ -45,9 +46,6 @@
     <t>Elemento</t>
   </si>
   <si>
-    <t>CTDAD</t>
-  </si>
-  <si>
     <t>Nº de pieza</t>
   </si>
   <si>
@@ -592,6 +590,18 @@
   </si>
   <si>
     <t>Sap</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>CTDAD de elementos</t>
+  </si>
+  <si>
+    <t>Proveedor</t>
+  </si>
+  <si>
+    <t>CTDADes</t>
   </si>
 </sst>
 </file>
@@ -805,8 +815,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{925C9BE9-A9EB-4A1C-9A13-A95B7A1791DD}" name="Inventor" displayName="Inventor" ref="A1:A9" totalsRowShown="0">
-  <autoFilter ref="A1:A9" xr:uid="{925C9BE9-A9EB-4A1C-9A13-A95B7A1791DD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{925C9BE9-A9EB-4A1C-9A13-A95B7A1791DD}" name="Inventor" displayName="Inventor" ref="A1:A12" totalsRowShown="0">
+  <autoFilter ref="A1:A12" xr:uid="{925C9BE9-A9EB-4A1C-9A13-A95B7A1791DD}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{47EC8DEA-A4E6-42D8-973F-ECB79AE8EDDD}" name="ColumnasExcelInventor"/>
   </tableColumns>
@@ -815,8 +825,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC948D35-CEB9-493D-8C0F-D0589F47B893}" name="RutasArcchivos" displayName="RutasArcchivos" ref="C1:D5" totalsRowShown="0">
-  <autoFilter ref="C1:D5" xr:uid="{AC948D35-CEB9-493D-8C0F-D0589F47B893}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC948D35-CEB9-493D-8C0F-D0589F47B893}" name="RutasArcchivos" displayName="RutasArcchivos" ref="A1:B5" totalsRowShown="0">
+  <autoFilter ref="A1:B5" xr:uid="{AC948D35-CEB9-493D-8C0F-D0589F47B893}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{F7664168-030D-4243-8197-46C70C8C3778}" name="RutasArchivo"/>
     <tableColumn id="2" xr3:uid="{643F1E84-BA01-472F-AD72-474A7C838473}" name="Direccion"/>
@@ -1110,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,85 +1133,131 @@
     <col min="4" max="4" width="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>181</v>
-      </c>
-      <c r="D3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{935998F6-83FC-49C8-B3C1-479AAF06E1CD}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3B3F05D-2A99-4E7A-97CA-3EF4495FA479}">
   <dimension ref="A1:E164"/>
   <sheetViews>
@@ -1218,24 +1274,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" t="s">
         <v>172</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>173</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" t="s">
         <v>174</v>
-      </c>
-      <c r="D1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1256,7 +1312,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1277,7 +1333,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1298,7 +1354,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1319,7 +1375,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1340,7 +1396,7 @@
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1361,7 +1417,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1382,7 +1438,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1403,7 +1459,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1424,7 +1480,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1445,7 +1501,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1466,7 +1522,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1487,7 +1543,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1508,7 +1564,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1529,7 +1585,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1550,7 +1606,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1571,7 +1627,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1592,7 +1648,7 @@
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1613,7 +1669,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1634,7 +1690,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1655,7 +1711,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1676,7 +1732,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1697,7 +1753,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1718,7 +1774,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1739,7 +1795,7 @@
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1760,7 +1816,7 @@
     </row>
     <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1781,7 +1837,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1802,7 +1858,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1823,7 +1879,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1844,7 +1900,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1865,7 +1921,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1886,7 +1942,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1907,7 +1963,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1928,7 +1984,7 @@
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1949,7 +2005,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1970,7 +2026,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -1991,7 +2047,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2012,7 +2068,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B39" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2033,7 +2089,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B40" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2054,7 +2110,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B41" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2075,7 +2131,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B42" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2096,7 +2152,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B43" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2117,7 +2173,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2138,7 +2194,7 @@
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2159,7 +2215,7 @@
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2180,7 +2236,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B47" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2199,51 +2255,51 @@
         <v>Tornillo de cuello cilíndrico</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" s="2">
+        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>8</v>
+      </c>
+      <c r="C48" s="2" t="str">
+        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
+        <v xml:space="preserve">DIN-513 </v>
+      </c>
+      <c r="D48" s="2">
+        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>53</v>
+      </c>
+      <c r="E48" s="2" t="str">
+        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
+        <v>Rosca dientes de sierra. Forma y dimensiones.</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B48" s="2">
-        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>8</v>
-      </c>
-      <c r="C48" s="2" t="str">
-        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
-        <v xml:space="preserve">DIN-513 </v>
-      </c>
-      <c r="D48" s="2">
+      <c r="B49" s="2">
+        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>8</v>
+      </c>
+      <c r="C49" s="2" t="str">
+        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
+        <v xml:space="preserve">DIN-514 </v>
+      </c>
+      <c r="D49" s="2">
         <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
         <v>53</v>
       </c>
-      <c r="E48" s="2" t="str">
+      <c r="E49" s="2" t="str">
         <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
         <v>Rosca dientes de sierra. Forma y dimensiones.</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="B49" s="2">
-        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>8</v>
-      </c>
-      <c r="C49" s="2" t="str">
-        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
-        <v xml:space="preserve">DIN-514 </v>
-      </c>
-      <c r="D49" s="2">
-        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>53</v>
-      </c>
-      <c r="E49" s="2" t="str">
-        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
-        <v>Rosca dientes de sierra. Forma y dimensiones.</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="B50" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2264,7 +2320,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B51" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2285,7 +2341,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B52" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2306,7 +2362,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B53" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2327,7 +2383,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2348,7 +2404,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B55" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2369,7 +2425,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B56" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2390,7 +2446,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2411,7 +2467,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B58" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2432,7 +2488,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B59" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2453,7 +2509,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B60" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2474,7 +2530,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B61" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2495,7 +2551,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B62" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2516,7 +2572,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B63" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2537,7 +2593,7 @@
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B64" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2558,7 +2614,7 @@
     </row>
     <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B65" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2579,7 +2635,7 @@
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B66" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2600,28 +2656,28 @@
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67" s="2">
+        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>8</v>
+      </c>
+      <c r="C67" s="2" t="str">
+        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
+        <v xml:space="preserve">DIN-912 </v>
+      </c>
+      <c r="D67" s="2">
+        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>71</v>
+      </c>
+      <c r="E67" s="2" t="str">
+        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
+        <v>Tornillos de cabeza cilíndrica con hexágono interior tipo Allen</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B67" s="2">
-        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>8</v>
-      </c>
-      <c r="C67" s="2" t="str">
-        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
-        <v xml:space="preserve">DIN-912 </v>
-      </c>
-      <c r="D67" s="2">
-        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>71</v>
-      </c>
-      <c r="E67" s="2" t="str">
-        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
-        <v>Tornillos de cabeza cilíndrica con hexágono interior tipo Allen</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="B68" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2642,7 +2698,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B69" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2663,7 +2719,7 @@
     </row>
     <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B70" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2684,7 +2740,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B71" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2705,7 +2761,7 @@
     </row>
     <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B72" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2726,7 +2782,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B73" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2747,7 +2803,7 @@
     </row>
     <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B74" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2768,7 +2824,7 @@
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B75" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2789,7 +2845,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B76" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2810,7 +2866,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B77" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2831,7 +2887,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B78" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2852,7 +2908,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B79" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2873,7 +2929,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B80" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2894,7 +2950,7 @@
     </row>
     <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B81" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2915,7 +2971,7 @@
     </row>
     <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B82" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2936,7 +2992,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B83" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2957,7 +3013,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B84" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2978,7 +3034,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B85" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -2999,7 +3055,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B86" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3020,7 +3076,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B87" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3041,7 +3097,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B88" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3062,7 +3118,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B89" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3083,7 +3139,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B90" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3104,7 +3160,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B91" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3125,7 +3181,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B92" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3146,7 +3202,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B93" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3167,7 +3223,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B94" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3188,7 +3244,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B95" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3209,7 +3265,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B96" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3230,7 +3286,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B97" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3251,7 +3307,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B98" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3272,7 +3328,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B99" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3293,7 +3349,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B100" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3314,7 +3370,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B101" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3335,7 +3391,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B102" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3356,7 +3412,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B103" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3377,7 +3433,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B104" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3398,7 +3454,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B105" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3419,7 +3475,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B106" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3440,7 +3496,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B107" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3461,7 +3517,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B108" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3482,7 +3538,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B109" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3503,7 +3559,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B110" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3524,7 +3580,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B111" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3545,7 +3601,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B112" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3566,7 +3622,7 @@
     </row>
     <row r="113" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B113" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3587,7 +3643,7 @@
     </row>
     <row r="114" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B114" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3608,7 +3664,7 @@
     </row>
     <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B115" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3629,7 +3685,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B116" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3650,28 +3706,28 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B117" s="2">
+        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>9</v>
+      </c>
+      <c r="C117" s="2" t="str">
+        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
+        <v xml:space="preserve">DIN-5463 </v>
+      </c>
+      <c r="D117" s="2">
+        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
+        <v>52</v>
+      </c>
+      <c r="E117" s="2" t="str">
+        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
+        <v>Acoplamiento de ejes nervados. Serie media.</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B117" s="2">
-        <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>9</v>
-      </c>
-      <c r="C117" s="2" t="str">
-        <f>LEFT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],DIN_TORNILLERIA[[#This Row],[Separacion]])</f>
-        <v xml:space="preserve">DIN-5463 </v>
-      </c>
-      <c r="D117" s="2">
-        <f>LEN(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
-        <v>52</v>
-      </c>
-      <c r="E117" s="2" t="str">
-        <f>RIGHT(DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]],(DIN_TORNILLERIA[[#This Row],[Longitud]]-DIN_TORNILLERIA[[#This Row],[Separacion]]))</f>
-        <v>Acoplamiento de ejes nervados. Serie media.</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="B118" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3692,7 +3748,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B119" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3713,7 +3769,7 @@
     </row>
     <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B120" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3734,7 +3790,7 @@
     </row>
     <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B121" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3755,7 +3811,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B122" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3776,7 +3832,7 @@
     </row>
     <row r="123" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B123" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3797,7 +3853,7 @@
     </row>
     <row r="124" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B124" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3818,7 +3874,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B125" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3839,7 +3895,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B126" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3860,7 +3916,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B127" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3881,7 +3937,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B128" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3902,7 +3958,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B129" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3923,7 +3979,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B130" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3944,7 +4000,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B131" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3965,7 +4021,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B132" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -3986,7 +4042,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B133" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4007,7 +4063,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B134" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4028,7 +4084,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B135" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4049,7 +4105,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B136" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4070,7 +4126,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B137" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4091,7 +4147,7 @@
     </row>
     <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B138" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4112,7 +4168,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B139" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4133,7 +4189,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B140" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4154,7 +4210,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B141" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4175,7 +4231,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B142" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4196,7 +4252,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B143" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4217,7 +4273,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B144" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4238,7 +4294,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B145" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4259,7 +4315,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B146" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4280,7 +4336,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B147" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4301,7 +4357,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B148" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4322,7 +4378,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B149" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4343,7 +4399,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B150" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4364,7 +4420,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B151" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4385,7 +4441,7 @@
     </row>
     <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B152" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4406,7 +4462,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B153" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4427,7 +4483,7 @@
     </row>
     <row r="154" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B154" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4448,7 +4504,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B155" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4469,7 +4525,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B156" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4490,7 +4546,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B157" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4511,7 +4567,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B158" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4532,7 +4588,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B159" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4553,7 +4609,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B160" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4574,7 +4630,7 @@
     </row>
     <row r="161" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B161" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4595,7 +4651,7 @@
     </row>
     <row r="162" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B162" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4616,7 +4672,7 @@
     </row>
     <row r="163" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B163" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>
@@ -4637,7 +4693,7 @@
     </row>
     <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B164" s="2">
         <f>FIND(" ",DIN_TORNILLERIA[[#This Row],[DIN Tornilleria]])</f>

</xml_diff>